<commit_message>
Update examplecontent.xlsx. Use german expressions and style reporoot row.
</commit_message>
<xml_diff>
--- a/opengever/examplecontent/data/examplecontent.xlsx
+++ b/opengever/examplecontent/data/examplecontent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="37340" windowHeight="23140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37480" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ordnungssystem" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="repository" localSheetId="0">Sheet1!$A$6:$W$47</definedName>
+    <definedName name="repository" localSheetId="0">Ordnungssystem!$A$6:$W$47</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="128">
   <si>
     <t>reference_number</t>
   </si>
@@ -119,24 +119,9 @@
     <t>Ordnungssystem</t>
   </si>
   <si>
-    <t>unprotected</t>
-  </si>
-  <si>
-    <t>privacy_layer_no</t>
-  </si>
-  <si>
-    <t>private</t>
-  </si>
-  <si>
-    <t>unchecked</t>
-  </si>
-  <si>
     <t>Strategie und Planung</t>
   </si>
   <si>
-    <t>archival worthy</t>
-  </si>
-  <si>
     <t>Berichtwesen</t>
   </si>
   <si>
@@ -149,9 +134,6 @@
     <t>Institutionelle Beziehungen</t>
   </si>
   <si>
-    <t>confidential</t>
-  </si>
-  <si>
     <t>Stellungnahmen... Mitberichte zuhanden Dritter</t>
   </si>
   <si>
@@ -167,9 +149,6 @@
     <t>Personaldossiers</t>
   </si>
   <si>
-    <t>privacy_layer_yes</t>
-  </si>
-  <si>
     <t>Lehrlinge und Praktika</t>
   </si>
   <si>
@@ -200,9 +179,6 @@
     <t>Administration</t>
   </si>
   <si>
-    <t>not archival worthy</t>
-  </si>
-  <si>
     <t>Kernbereich 1</t>
   </si>
   <si>
@@ -212,9 +188,6 @@
     <t>Kernbereich 1b</t>
   </si>
   <si>
-    <t>archival worthy with sampling</t>
-  </si>
-  <si>
     <t>Kernbereich 2</t>
   </si>
   <si>
@@ -441,13 +414,40 @@
   </si>
   <si>
     <t>responsible_org_unit</t>
+  </si>
+  <si>
+    <t>Nicht klassifiziert</t>
+  </si>
+  <si>
+    <t>Vertraulich</t>
+  </si>
+  <si>
+    <t>Keine Datenschutzstufe</t>
+  </si>
+  <si>
+    <t>Enthält schützenswerte Personendaten</t>
+  </si>
+  <si>
+    <t>Nicht öffentlich</t>
+  </si>
+  <si>
+    <t>Nicht geprüft</t>
+  </si>
+  <si>
+    <t>Archivwürdig</t>
+  </si>
+  <si>
+    <t>Nicht archivwürdig</t>
+  </si>
+  <si>
+    <t>Sampling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -501,8 +501,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,6 +541,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,10 +586,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -592,19 +645,12 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -612,6 +658,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -637,8 +686,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -976,19 +1052,19 @@
   <dimension ref="A1:V47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="K40" sqref="C40:K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.33203125" customWidth="1"/>
-    <col min="3" max="3" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1640625" customWidth="1"/>
+    <col min="7" max="7" width="34.5" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
     <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.6640625" bestFit="1" customWidth="1"/>
@@ -1031,93 +1107,93 @@
       <c r="V2"/>
     </row>
     <row r="3" spans="1:22" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A3" s="22"/>
-      <c r="B3" s="24" t="s">
+      <c r="A3" s="24"/>
+      <c r="B3" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="M3" s="20" t="s">
         <v>79</v>
-      </c>
-      <c r="D3" s="27"/>
-      <c r="E3" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="L3" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="M3" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="N3" s="10"/>
       <c r="O3" s="10"/>
       <c r="P3" s="11"/>
-      <c r="Q3" s="15" t="s">
+      <c r="Q3" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="S3" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="V3"/>
+    </row>
+    <row r="4" spans="1:22" s="5" customFormat="1" ht="77.25" customHeight="1">
+      <c r="A4" s="25"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="31"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="R3" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="S3" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="T3" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="U3" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="V3"/>
-    </row>
-    <row r="4" spans="1:22" s="5" customFormat="1" ht="77.25" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
       <c r="V4"/>
     </row>
     <row r="5" spans="1:22" ht="20" hidden="1" customHeight="1">
@@ -1128,7 +1204,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
         <v>2</v>
@@ -1183,313 +1259,337 @@
       </c>
     </row>
     <row r="6" spans="1:22">
+      <c r="A6" s="16"/>
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6">
-        <v>10</v>
-      </c>
-      <c r="K6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6">
-        <v>30</v>
-      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
       <c r="N6" s="1">
         <v>40452</v>
+      </c>
+      <c r="O6" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="14" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
+        <v>50</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H7" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I7">
         <v>10</v>
       </c>
       <c r="K7" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="M7">
         <v>30</v>
       </c>
       <c r="N7" s="1">
         <v>40452</v>
+      </c>
+      <c r="O7" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="14" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
         <v>20</v>
       </c>
+      <c r="F8" s="18" t="s">
+        <v>119</v>
+      </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I8">
         <v>10</v>
       </c>
       <c r="K8" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="M8">
         <v>30</v>
       </c>
       <c r="N8" s="1">
         <v>40452</v>
+      </c>
+      <c r="O8" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="14" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H9" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I9">
         <v>10</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="M9">
         <v>30</v>
       </c>
       <c r="N9" s="1">
         <v>40452</v>
+      </c>
+      <c r="O9" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="14" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I10">
         <v>10</v>
       </c>
       <c r="K10" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="M10">
         <v>30</v>
       </c>
       <c r="N10" s="1">
         <v>40452</v>
+      </c>
+      <c r="O10" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="14" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H11" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I11">
         <v>10</v>
       </c>
       <c r="K11" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="M11">
         <v>30</v>
       </c>
       <c r="N11" s="1">
         <v>40452</v>
+      </c>
+      <c r="O11" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="14" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H12" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I12">
         <v>10</v>
       </c>
       <c r="K12" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="M12">
         <v>30</v>
       </c>
       <c r="N12" s="1">
         <v>40452</v>
+      </c>
+      <c r="O12" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="14" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" t="s">
-        <v>20</v>
+        <v>67</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H13" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I13">
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="M13">
         <v>30</v>
       </c>
       <c r="N13" s="1">
         <v>40452</v>
+      </c>
+      <c r="O13" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="14" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H14" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I14">
         <v>10</v>
       </c>
       <c r="K14" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="M14">
         <v>30</v>
       </c>
       <c r="N14" s="1">
         <v>40452</v>
+      </c>
+      <c r="O14" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="14" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H15" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I15">
         <v>10</v>
       </c>
       <c r="K15" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="M15">
         <v>30</v>
       </c>
       <c r="N15" s="1">
         <v>40452</v>
+      </c>
+      <c r="O15" s="1">
+        <v>51440</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="14" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" t="s">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H16" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I16">
         <v>10</v>
       </c>
       <c r="K16" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="M16">
         <v>30</v>
@@ -1497,28 +1597,31 @@
       <c r="N16" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="14" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" t="s">
-        <v>20</v>
+        <v>65</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G17" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H17" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I17">
         <v>10</v>
       </c>
       <c r="K17" t="s">
-        <v>23</v>
+        <v>124</v>
       </c>
       <c r="M17">
         <v>30</v>
@@ -1526,28 +1629,31 @@
       <c r="N17" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="O17" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="14" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>119</v>
       </c>
       <c r="G18" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="H18" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I18">
         <v>10</v>
       </c>
       <c r="K18" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="M18">
         <v>30</v>
@@ -1555,28 +1661,31 @@
       <c r="N18" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="O18" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="14" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="G19" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="H19" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I19">
         <v>10</v>
       </c>
       <c r="K19" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="M19">
         <v>100</v>
@@ -1584,550 +1693,607 @@
       <c r="N19" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" t="s">
+        <v>121</v>
+      </c>
+      <c r="H20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20">
+        <v>10</v>
+      </c>
+      <c r="K20" t="s">
+        <v>125</v>
+      </c>
+      <c r="M20">
+        <v>30</v>
+      </c>
+      <c r="N20" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O20" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" t="s">
+        <v>121</v>
+      </c>
+      <c r="H21" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21">
+        <v>10</v>
+      </c>
+      <c r="K21" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M21">
+        <v>30</v>
+      </c>
+      <c r="N21" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O21" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="K22" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M22">
+        <v>30</v>
+      </c>
+      <c r="N22" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O22" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G23" t="s">
+        <v>121</v>
+      </c>
+      <c r="H23" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="K23" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M23">
+        <v>30</v>
+      </c>
+      <c r="N23" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O23" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
+      </c>
+      <c r="K24" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M24">
+        <v>30</v>
+      </c>
+      <c r="N24" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O24" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" t="s">
+        <v>121</v>
+      </c>
+      <c r="H25" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="K25" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M25">
+        <v>30</v>
+      </c>
+      <c r="N25" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O25" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G26" t="s">
+        <v>121</v>
+      </c>
+      <c r="H26" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26">
+        <v>10</v>
+      </c>
+      <c r="K26" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M26">
+        <v>30</v>
+      </c>
+      <c r="N26" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O26" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" t="s">
+        <v>121</v>
+      </c>
+      <c r="H27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27">
+        <v>10</v>
+      </c>
+      <c r="K27" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M27">
+        <v>30</v>
+      </c>
+      <c r="N27" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O27" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" t="s">
+        <v>121</v>
+      </c>
+      <c r="H28" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28">
+        <v>10</v>
+      </c>
+      <c r="K28" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M28">
+        <v>30</v>
+      </c>
+      <c r="N28" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O28" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G29" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29">
+        <v>10</v>
+      </c>
+      <c r="K29" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M29">
+        <v>30</v>
+      </c>
+      <c r="N29" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O29" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G30" t="s">
+        <v>121</v>
+      </c>
+      <c r="H30" t="s">
+        <v>123</v>
+      </c>
+      <c r="I30">
+        <v>10</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M30">
+        <v>30</v>
+      </c>
+      <c r="N30" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O30" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G31" t="s">
+        <v>121</v>
+      </c>
+      <c r="H31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M31">
+        <v>30</v>
+      </c>
+      <c r="N31" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O31" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I20">
-        <v>10</v>
-      </c>
-      <c r="K20" t="s">
-        <v>25</v>
-      </c>
-      <c r="M20">
-        <v>30</v>
-      </c>
-      <c r="N20" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B32" t="s">
         <v>37</v>
       </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21">
-        <v>10</v>
-      </c>
-      <c r="K21" t="s">
-        <v>23</v>
-      </c>
-      <c r="M21">
-        <v>30</v>
-      </c>
-      <c r="N21" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="F32" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G32" t="s">
+        <v>121</v>
+      </c>
+      <c r="H32" t="s">
+        <v>123</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M32">
+        <v>30</v>
+      </c>
+      <c r="N32" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O32" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
         <v>38</v>
       </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" t="s">
-        <v>22</v>
-      </c>
-      <c r="I22">
-        <v>10</v>
-      </c>
-      <c r="K22" t="s">
-        <v>23</v>
-      </c>
-      <c r="M22">
-        <v>30</v>
-      </c>
-      <c r="N22" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23">
-        <v>10</v>
-      </c>
-      <c r="K23" t="s">
-        <v>23</v>
-      </c>
-      <c r="M23">
-        <v>30</v>
-      </c>
-      <c r="N23" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="F33" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G33" t="s">
+        <v>121</v>
+      </c>
+      <c r="H33" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M33">
+        <v>30</v>
+      </c>
+      <c r="N33" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O33" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
         <v>39</v>
       </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24">
-        <v>10</v>
-      </c>
-      <c r="K24" t="s">
-        <v>23</v>
-      </c>
-      <c r="M24">
-        <v>30</v>
-      </c>
-      <c r="N24" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="A25" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="F34" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G34" t="s">
+        <v>121</v>
+      </c>
+      <c r="H34" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34">
+        <v>10</v>
+      </c>
+      <c r="K34" t="s">
+        <v>126</v>
+      </c>
+      <c r="M34">
+        <v>30</v>
+      </c>
+      <c r="N34" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O34" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
         <v>40</v>
       </c>
-      <c r="F25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25">
-        <v>10</v>
-      </c>
-      <c r="K25" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25">
-        <v>30</v>
-      </c>
-      <c r="N25" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="A26" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="F35" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" t="s">
+        <v>121</v>
+      </c>
+      <c r="H35" t="s">
+        <v>123</v>
+      </c>
+      <c r="I35">
+        <v>10</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="M35">
+        <v>30</v>
+      </c>
+      <c r="N35" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O35" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="F26" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26">
-        <v>10</v>
-      </c>
-      <c r="K26" t="s">
-        <v>23</v>
-      </c>
-      <c r="M26">
-        <v>30</v>
-      </c>
-      <c r="N26" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="A27" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="F36" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" t="s">
+        <v>121</v>
+      </c>
+      <c r="H36" t="s">
+        <v>123</v>
+      </c>
+      <c r="I36">
+        <v>10</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="M36">
+        <v>30</v>
+      </c>
+      <c r="N36" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O36" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
         <v>42</v>
       </c>
-      <c r="F27" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" t="s">
-        <v>21</v>
-      </c>
-      <c r="H27" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27">
-        <v>10</v>
-      </c>
-      <c r="K27" t="s">
-        <v>23</v>
-      </c>
-      <c r="M27">
-        <v>30</v>
-      </c>
-      <c r="N27" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="A28" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" t="s">
-        <v>21</v>
-      </c>
-      <c r="H28" t="s">
-        <v>22</v>
-      </c>
-      <c r="I28">
-        <v>10</v>
-      </c>
-      <c r="K28" t="s">
-        <v>23</v>
-      </c>
-      <c r="M28">
-        <v>30</v>
-      </c>
-      <c r="N28" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="A29" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29">
-        <v>10</v>
-      </c>
-      <c r="K29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M29">
-        <v>30</v>
-      </c>
-      <c r="N29" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="A30" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="F37" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G37" t="s">
+        <v>121</v>
+      </c>
+      <c r="H37" t="s">
+        <v>123</v>
+      </c>
+      <c r="I37">
+        <v>10</v>
+      </c>
+      <c r="K37" t="s">
+        <v>127</v>
+      </c>
+      <c r="M37">
+        <v>30</v>
+      </c>
+      <c r="N37" s="1">
+        <v>40452</v>
+      </c>
+      <c r="O37" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
+      <c r="A38" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
         <v>43</v>
       </c>
-      <c r="F30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" t="s">
-        <v>22</v>
-      </c>
-      <c r="I30">
-        <v>10</v>
-      </c>
-      <c r="K30" t="s">
-        <v>23</v>
-      </c>
-      <c r="M30">
-        <v>30</v>
-      </c>
-      <c r="N30" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="A31" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" t="s">
-        <v>77</v>
-      </c>
-      <c r="F31" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31">
-        <v>10</v>
-      </c>
-      <c r="K31" t="s">
-        <v>23</v>
-      </c>
-      <c r="M31">
-        <v>30</v>
-      </c>
-      <c r="N31" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="A32" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G32" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" t="s">
-        <v>22</v>
-      </c>
-      <c r="I32">
-        <v>10</v>
-      </c>
-      <c r="K32" t="s">
-        <v>23</v>
-      </c>
-      <c r="M32">
-        <v>30</v>
-      </c>
-      <c r="N32" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
-      <c r="A33" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="B33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G33" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" t="s">
-        <v>22</v>
-      </c>
-      <c r="I33">
-        <v>10</v>
-      </c>
-      <c r="K33" t="s">
-        <v>23</v>
-      </c>
-      <c r="M33">
-        <v>30</v>
-      </c>
-      <c r="N33" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
-      <c r="A34" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B34" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" t="s">
-        <v>21</v>
-      </c>
-      <c r="H34" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34">
-        <v>10</v>
-      </c>
-      <c r="K34" t="s">
-        <v>47</v>
-      </c>
-      <c r="M34">
-        <v>30</v>
-      </c>
-      <c r="N34" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
-      <c r="A35" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="B35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" t="s">
-        <v>20</v>
-      </c>
-      <c r="G35" t="s">
-        <v>21</v>
-      </c>
-      <c r="H35" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35">
-        <v>10</v>
-      </c>
-      <c r="K35" t="s">
-        <v>23</v>
-      </c>
-      <c r="M35">
-        <v>30</v>
-      </c>
-      <c r="N35" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
-      <c r="A36" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="B36" t="s">
-        <v>49</v>
-      </c>
-      <c r="F36" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" t="s">
-        <v>21</v>
-      </c>
-      <c r="H36" t="s">
-        <v>22</v>
-      </c>
-      <c r="I36">
-        <v>10</v>
-      </c>
-      <c r="K36" t="s">
-        <v>25</v>
-      </c>
-      <c r="M36">
-        <v>30</v>
-      </c>
-      <c r="N36" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
-      <c r="A37" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="B37" t="s">
-        <v>50</v>
-      </c>
-      <c r="F37" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37" t="s">
-        <v>21</v>
-      </c>
-      <c r="H37" t="s">
-        <v>22</v>
-      </c>
-      <c r="I37">
-        <v>10</v>
-      </c>
-      <c r="K37" t="s">
-        <v>51</v>
-      </c>
-      <c r="M37">
-        <v>30</v>
-      </c>
-      <c r="N37" s="1">
-        <v>40452</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
-      <c r="A38" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
       <c r="F38" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="G38" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="H38" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I38">
         <v>10</v>
       </c>
-      <c r="K38" t="s">
-        <v>23</v>
+      <c r="K38" s="19" t="s">
+        <v>124</v>
       </c>
       <c r="M38">
         <v>100</v>
@@ -2135,28 +2301,31 @@
       <c r="N38" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="O38" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" s="14" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="G39" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="H39" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I39">
         <v>10</v>
       </c>
-      <c r="K39" t="s">
-        <v>25</v>
+      <c r="K39" s="19" t="s">
+        <v>125</v>
       </c>
       <c r="M39">
         <v>100</v>
@@ -2164,28 +2333,31 @@
       <c r="N39" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="O39" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" s="14" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="F40" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="G40" t="s">
-        <v>36</v>
+        <v>122</v>
       </c>
       <c r="H40" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I40">
         <v>10</v>
       </c>
       <c r="K40" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="M40">
         <v>100</v>
@@ -2193,28 +2365,31 @@
       <c r="N40" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="O40" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" s="14" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>55</v>
-      </c>
-      <c r="F41" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" t="s">
-        <v>21</v>
+        <v>46</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="H41" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I41">
         <v>10</v>
       </c>
-      <c r="K41" t="s">
-        <v>23</v>
+      <c r="K41" s="19" t="s">
+        <v>124</v>
       </c>
       <c r="M41">
         <v>30</v>
@@ -2222,28 +2397,31 @@
       <c r="N41" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="42" spans="1:14">
+      <c r="O41" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42" s="14" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F42" t="s">
-        <v>20</v>
-      </c>
-      <c r="G42" t="s">
-        <v>21</v>
+        <v>47</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="H42" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I42">
         <v>10</v>
       </c>
       <c r="K42" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="M42">
         <v>30</v>
@@ -2251,28 +2429,31 @@
       <c r="N42" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="O42" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43" s="14" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43" t="s">
-        <v>21</v>
+        <v>48</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="H43" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I43">
         <v>10</v>
       </c>
       <c r="K43" t="s">
-        <v>47</v>
+        <v>126</v>
       </c>
       <c r="M43">
         <v>30</v>
@@ -2280,28 +2461,31 @@
       <c r="N43" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="44" spans="1:14">
+      <c r="O43" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44" s="14" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>58</v>
-      </c>
-      <c r="F44" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44" t="s">
-        <v>21</v>
+        <v>49</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="H44" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I44">
         <v>10</v>
       </c>
-      <c r="K44" t="s">
-        <v>25</v>
+      <c r="K44" s="19" t="s">
+        <v>125</v>
       </c>
       <c r="M44">
         <v>30</v>
@@ -2309,28 +2493,31 @@
       <c r="N44" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="45" spans="1:14">
+      <c r="O44" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45" s="14" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
-      </c>
-      <c r="F45" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" t="s">
-        <v>21</v>
+        <v>40</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="H45" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I45">
         <v>10</v>
       </c>
-      <c r="K45" t="s">
-        <v>25</v>
+      <c r="K45" s="19" t="s">
+        <v>125</v>
       </c>
       <c r="M45">
         <v>30</v>
@@ -2338,67 +2525,84 @@
       <c r="N45" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="46" spans="1:14">
+      <c r="O45" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H46" t="s">
+        <v>123</v>
+      </c>
+      <c r="I46">
+        <v>10</v>
+      </c>
+      <c r="K46" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B46" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" t="s">
-        <v>20</v>
-      </c>
-      <c r="G46" t="s">
-        <v>21</v>
-      </c>
-      <c r="H46" t="s">
-        <v>22</v>
-      </c>
-      <c r="I46">
-        <v>10</v>
-      </c>
-      <c r="K46" t="s">
-        <v>25</v>
-      </c>
       <c r="M46">
         <v>30</v>
       </c>
       <c r="N46" s="1">
         <v>40452</v>
       </c>
-    </row>
-    <row r="47" spans="1:14">
+      <c r="O46" s="1">
+        <v>51440</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47" s="14" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" t="s">
-        <v>20</v>
-      </c>
-      <c r="G47" t="s">
-        <v>21</v>
+        <v>46</v>
+      </c>
+      <c r="F47" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>121</v>
       </c>
       <c r="H47" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
       <c r="I47">
         <v>10</v>
       </c>
-      <c r="K47" t="s">
-        <v>25</v>
+      <c r="K47" s="19" t="s">
+        <v>125</v>
       </c>
       <c r="M47">
         <v>30</v>
       </c>
       <c r="N47" s="1">
         <v>40452</v>
+      </c>
+      <c r="O47" s="1">
+        <v>51440</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="M3:M4"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="J3:J4"/>
@@ -2408,16 +2612,9 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:L4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="S3:S4"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="M3:M4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>